<commit_message>
Sql and ads update
new AD links added,
travel packages for davao in sql
</commit_message>
<xml_diff>
--- a/classifiedAds.xlsx
+++ b/classifiedAds.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>RealBreeze</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>http://www.cebuclassifieds.com/ad/1818436-samal-island-hopping-davao-del-sur</t>
+  </si>
+  <si>
+    <t>http://davao.locanto.ph/ID_1709333145/Davao-Budget-Tour-3D-2N.html</t>
+  </si>
+  <si>
+    <t>http://davao.locanto.ph/ID_1709385452/Mountain-Tour-Package.html</t>
   </si>
 </sst>
 </file>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,8 +525,10 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="6" width="43.7109375" customWidth="1"/>
-    <col min="7" max="7" width="71.5703125" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="103.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -623,6 +631,9 @@
       <c r="F9" t="s">
         <v>13</v>
       </c>
+      <c r="H9" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -654,6 +665,9 @@
       <c r="F11" t="s">
         <v>13</v>
       </c>
+      <c r="H11" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
@@ -727,25 +741,35 @@
         <v>37</v>
       </c>
     </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="G19" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="5" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="5" t="s">
         <v>41</v>
       </c>
     </row>
@@ -758,8 +782,10 @@
     <hyperlink ref="G15" r:id="rId5"/>
     <hyperlink ref="G16" r:id="rId6"/>
     <hyperlink ref="G17" r:id="rId7"/>
-    <hyperlink ref="G19" r:id="rId8"/>
-    <hyperlink ref="G20" r:id="rId9"/>
+    <hyperlink ref="G21" r:id="rId8"/>
+    <hyperlink ref="G22" r:id="rId9"/>
+    <hyperlink ref="G18" r:id="rId10"/>
+    <hyperlink ref="G19" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New ads and AdsList
</commit_message>
<xml_diff>
--- a/classifiedAds.xlsx
+++ b/classifiedAds.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
   <si>
     <t>RealBreeze</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>https://davao-city-das-ph.global-free-classified-ads.com/listings/pearl-farm-beach-resort-it8984814.html</t>
+  </si>
+  <si>
+    <t>https://davao-city-das-ph.global-free-classified-ads.com/listings/camiguin-tour-package-philippines-it8993666.html</t>
+  </si>
+  <si>
+    <t>https://davao-city-das-ph.global-free-classified-ads.com/listings/samal-island-hopping-it8993758.html</t>
   </si>
 </sst>
 </file>
@@ -566,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="F6" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,10 +821,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
       <c r="E20" s="7"/>
+      <c r="G20" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
@@ -827,43 +833,45 @@
       </c>
       <c r="E21" s="7"/>
       <c r="G21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="G22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="6" t="s">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G24" s="6" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -871,7 +879,7 @@
         <v>29</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,7 +887,7 @@
         <v>29</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -887,7 +895,7 @@
         <v>29</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -895,7 +903,7 @@
         <v>29</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -903,7 +911,7 @@
         <v>29</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -911,7 +919,7 @@
         <v>29</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -919,7 +927,7 @@
         <v>29</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -927,7 +935,7 @@
         <v>29</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -935,7 +943,7 @@
         <v>29</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -943,32 +951,32 @@
         <v>29</v>
       </c>
       <c r="G34" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B35" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -976,7 +984,7 @@
         <v>29</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -984,7 +992,7 @@
         <v>29</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -992,7 +1000,7 @@
         <v>29</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1000,7 +1008,7 @@
         <v>29</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1008,6 +1016,14 @@
         <v>29</v>
       </c>
       <c r="G41" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New ads on Adsriver
</commit_message>
<xml_diff>
--- a/classifiedAds.xlsx
+++ b/classifiedAds.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="84">
   <si>
     <t>RealBreeze</t>
   </si>
@@ -247,6 +247,30 @@
   </si>
   <si>
     <t>http://www.adsriver.com/34/posts/20-Travel-Tickets/377-Other-Travel-Ads/987572-Davao-to-Lake-Agco-Mt-Apo-.html</t>
+  </si>
+  <si>
+    <t>http://www.adsriver.com/34/posts/20-Travel-Tickets/376--Vacation-Rentals/988030-Davao-Country-Side-Tour-.html</t>
+  </si>
+  <si>
+    <t>http://www.adsriver.com/34/posts/20-Travel-Tickets/377-Other-Travel-Ads/988031-Surigao-Tour-Package-.html</t>
+  </si>
+  <si>
+    <t>http://www.adsriver.com/34/posts/20-Travel-Tickets/377-Other-Travel-Ads/988032-Camiguin-Tour-Package.html</t>
+  </si>
+  <si>
+    <t>http://www.adsriver.com/34/posts/20-Travel-Tickets/377-Other-Travel-Ads/988034-Mati-Davao-Oriental-.html</t>
+  </si>
+  <si>
+    <t>http://www.adsriver.com/34/posts/20-Travel-Tickets/377-Other-Travel-Ads/988036-Davao-City-Tour.html</t>
+  </si>
+  <si>
+    <t>http://www.adsriver.com/34/posts/20-Travel-Tickets/377-Other-Travel-Ads/988037-Davao-White-Water-Rafting.html</t>
+  </si>
+  <si>
+    <t>http://www.adsriver.com/34/posts/20-Travel-Tickets/376--Vacation-Rentals/988040-Pearl-Farm-Beach-Resort.html</t>
+  </si>
+  <si>
+    <t>http://www.adsriver.com/34/posts/20-Travel-Tickets/376--Vacation-Rentals/988041-Samal-Island-Hopping-Package-.html</t>
   </si>
 </sst>
 </file>
@@ -608,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:F30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,84 +1031,84 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="B36" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>32</v>
+      <c r="G36" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>33</v>
+      <c r="G37" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>29</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>34</v>
+      <c r="G38" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>29</v>
       </c>
-      <c r="G39" s="6" t="s">
-        <v>35</v>
+      <c r="G39" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>40</v>
+      <c r="G40" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>29</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>41</v>
+      <c r="G41" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>29</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>42</v>
+      <c r="G42" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>29</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>43</v>
+      <c r="G43" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="B44" t="s">
         <v>29</v>
       </c>
+      <c r="E44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" t="s">
+        <v>13</v>
+      </c>
       <c r="G44" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1092,7 +1116,7 @@
         <v>29</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1100,7 +1124,7 @@
         <v>29</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1108,7 +1132,7 @@
         <v>29</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -1116,7 +1140,7 @@
         <v>29</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -1124,7 +1148,7 @@
         <v>29</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1132,7 +1156,7 @@
         <v>29</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1140,7 +1164,7 @@
         <v>29</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1148,24 +1172,15 @@
         <v>29</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="B53" t="s">
         <v>29</v>
       </c>
-      <c r="E53" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F53" t="s">
-        <v>37</v>
-      </c>
       <c r="G53" s="6" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1173,7 +1188,7 @@
         <v>29</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1181,7 +1196,7 @@
         <v>29</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1189,7 +1204,7 @@
         <v>29</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1197,7 +1212,7 @@
         <v>29</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,7 +1220,7 @@
         <v>29</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -1213,14 +1228,95 @@
         <v>29</v>
       </c>
       <c r="G59" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>29</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B61" t="s">
+        <v>29</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>29</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>29</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>29</v>
+      </c>
+      <c r="G67" s="6" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E12" r:id="rId1"/>
+    <hyperlink ref="G36" r:id="rId2"/>
+    <hyperlink ref="G37" r:id="rId3"/>
+    <hyperlink ref="G40" r:id="rId4"/>
+    <hyperlink ref="G38" r:id="rId5"/>
+    <hyperlink ref="G39" r:id="rId6"/>
+    <hyperlink ref="G41" r:id="rId7"/>
+    <hyperlink ref="G42" r:id="rId8"/>
+    <hyperlink ref="G43" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>